<commit_message>
gant diagramm Prozent der Aufgaben aktualisiert
</commit_message>
<xml_diff>
--- a/GanttDiagramm.xlsx
+++ b/GanttDiagramm.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0026B08-A9DC-4044-842B-7DDCF7072050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9753C46A-C220-4941-AC89-298835080C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="415" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="415" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="65">
   <si>
     <t>INFORMATIONEN ZU DIESEM GANTT-DIAGRAMM</t>
   </si>
@@ -269,24 +269,6 @@
   </si>
   <si>
     <t>Fazit/Ausblick</t>
-  </si>
-  <si>
-    <t>TITEL 6</t>
-  </si>
-  <si>
-    <t>Aufgabe 11</t>
-  </si>
-  <si>
-    <t>Aufgabe 12</t>
-  </si>
-  <si>
-    <t>Aufgabe 13</t>
-  </si>
-  <si>
-    <t>Aufgabe 14</t>
-  </si>
-  <si>
-    <t>Aufgabe 15</t>
   </si>
 </sst>
 </file>
@@ -2851,19 +2833,19 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="8" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="8" customWidth="1"/>
-    <col min="3" max="5" width="40.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="4.7265625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="2.7265625" style="8" customWidth="1"/>
+    <col min="3" max="5" width="40.7265625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="2.7265625" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="7" customFormat="1" ht="28.5" x14ac:dyDescent="0.6">
       <c r="D1" s="107"/>
     </row>
-    <row r="2" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="50.15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="7"/>
       <c r="B2" s="113"/>
       <c r="C2" s="126" t="s">
@@ -2880,7 +2862,7 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A3" s="7"/>
       <c r="B3" s="108"/>
       <c r="C3" s="109"/>
@@ -2895,7 +2877,7 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" s="8" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="7"/>
       <c r="B4" s="108"/>
       <c r="C4" s="127" t="s">
@@ -2912,7 +2894,7 @@
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" ht="193.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" s="8" customFormat="1" ht="193.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="7"/>
       <c r="B5" s="108"/>
       <c r="C5" s="127" t="s">
@@ -2929,7 +2911,7 @@
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="96.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" s="111"/>
       <c r="C6" s="111"/>
@@ -2937,15 +2919,15 @@
       <c r="E6" s="111"/>
       <c r="F6" s="111"/>
     </row>
-    <row r="7" spans="1:13" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="50.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
     </row>
-    <row r="9" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="90" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -2953,51 +2935,51 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="D19" s="8"/>
@@ -3025,22 +3007,22 @@
       <selection activeCell="BT11" sqref="BT11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="64" width="3.5703125" customWidth="1"/>
-    <col min="65" max="65" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" customWidth="1"/>
+    <col min="9" max="64" width="3.54296875" customWidth="1"/>
+    <col min="65" max="65" width="2.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="129" t="s">
         <v>3</v>
@@ -3109,7 +3091,7 @@
       <c r="BL2" s="67"/>
       <c r="BM2" s="67"/>
     </row>
-    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="68"/>
       <c r="C3" s="69"/>
@@ -3123,7 +3105,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="72" t="s">
         <v>4</v>
@@ -3177,7 +3159,7 @@
       <c r="AO4" s="128"/>
       <c r="AP4" s="128"/>
     </row>
-    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -3191,14 +3173,14 @@
       <c r="G5" s="75"/>
       <c r="H5" s="75"/>
     </row>
-    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="10"/>
       <c r="B6" s="79" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="80" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Meilensteine4352[Start])=0,TODAY(),B11(Meilensteine4352[Start])),TODAY())</f>
-        <v>45211</v>
+        <v>45298</v>
       </c>
       <c r="D6" s="81"/>
       <c r="E6" s="75"/>
@@ -3207,7 +3189,7 @@
       <c r="H6" s="75"/>
       <c r="I6" s="91" t="str">
         <f ca="1">TEXT(I7,"MMMM")</f>
-        <v>Oktober</v>
+        <v>Januar</v>
       </c>
       <c r="J6" s="91"/>
       <c r="K6" s="91"/>
@@ -3237,7 +3219,7 @@
       <c r="AC6" s="91"/>
       <c r="AD6" s="91" t="str">
         <f ca="1">IF(OR(TEXT(AD7,"MMMM")=W6,TEXT(AD7,"MMMM")=P6,TEXT(AD7,"MMMM")=I6),"",TEXT(AD7,"MMMM"))</f>
-        <v>November</v>
+        <v/>
       </c>
       <c r="AE6" s="91"/>
       <c r="AF6" s="91"/>
@@ -3247,7 +3229,7 @@
       <c r="AJ6" s="91"/>
       <c r="AK6" s="91" t="str">
         <f ca="1">IF(OR(TEXT(AK7,"MMMM")=AD6,TEXT(AK7,"MMMM")=W6,TEXT(AK7,"MMMM")=P6,TEXT(AK7,"MMMM")=I6),"",TEXT(AK7,"MMMM"))</f>
-        <v/>
+        <v>Februar</v>
       </c>
       <c r="AL6" s="91"/>
       <c r="AM6" s="91"/>
@@ -3277,7 +3259,7 @@
       <c r="BE6" s="90"/>
       <c r="BF6" s="90" t="str">
         <f ca="1">IF(OR(TEXT(BF7,"MMMM")=AY6,TEXT(BF7,"MMMM")=AR6,TEXT(BF7,"MMMM")=AK6,TEXT(BF7,"MMMM")=AD6),"",TEXT(BF7,"MMMM"))</f>
-        <v>Dezember</v>
+        <v/>
       </c>
       <c r="BG6" s="90"/>
       <c r="BH6" s="90"/>
@@ -3286,7 +3268,7 @@
       <c r="BK6" s="90"/>
       <c r="BL6" s="90"/>
     </row>
-    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="79" t="s">
         <v>14</v>
@@ -3301,230 +3283,230 @@
       <c r="H7" s="83"/>
       <c r="I7" s="98">
         <f ca="1">IFERROR(Projekt_Start+Scrollschrittweite,TODAY())</f>
-        <v>45212</v>
+        <v>45299</v>
       </c>
       <c r="J7" s="99">
         <f ca="1">I7+1</f>
-        <v>45213</v>
+        <v>45300</v>
       </c>
       <c r="K7" s="99">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45214</v>
+        <v>45301</v>
       </c>
       <c r="L7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45215</v>
+        <v>45302</v>
       </c>
       <c r="M7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45216</v>
+        <v>45303</v>
       </c>
       <c r="N7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="O7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45218</v>
+        <v>45305</v>
       </c>
       <c r="P7" s="99">
         <f ca="1">O7+1</f>
-        <v>45219</v>
+        <v>45306</v>
       </c>
       <c r="Q7" s="99">
         <f ca="1">P7+1</f>
-        <v>45220</v>
+        <v>45307</v>
       </c>
       <c r="R7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45221</v>
+        <v>45308</v>
       </c>
       <c r="S7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45222</v>
+        <v>45309</v>
       </c>
       <c r="T7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45223</v>
+        <v>45310</v>
       </c>
       <c r="U7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45224</v>
+        <v>45311</v>
       </c>
       <c r="V7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45225</v>
+        <v>45312</v>
       </c>
       <c r="W7" s="99">
         <f ca="1">V7+1</f>
-        <v>45226</v>
+        <v>45313</v>
       </c>
       <c r="X7" s="99">
         <f ca="1">W7+1</f>
-        <v>45227</v>
+        <v>45314</v>
       </c>
       <c r="Y7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45228</v>
+        <v>45315</v>
       </c>
       <c r="Z7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45229</v>
+        <v>45316</v>
       </c>
       <c r="AA7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45230</v>
+        <v>45317</v>
       </c>
       <c r="AB7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45231</v>
+        <v>45318</v>
       </c>
       <c r="AC7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45232</v>
+        <v>45319</v>
       </c>
       <c r="AD7" s="99">
         <f ca="1">AC7+1</f>
-        <v>45233</v>
+        <v>45320</v>
       </c>
       <c r="AE7" s="99">
         <f ca="1">AD7+1</f>
-        <v>45234</v>
+        <v>45321</v>
       </c>
       <c r="AF7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45235</v>
+        <v>45322</v>
       </c>
       <c r="AG7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45236</v>
+        <v>45323</v>
       </c>
       <c r="AH7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45237</v>
+        <v>45324</v>
       </c>
       <c r="AI7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45238</v>
+        <v>45325</v>
       </c>
       <c r="AJ7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45239</v>
+        <v>45326</v>
       </c>
       <c r="AK7" s="99">
         <f ca="1">AJ7+1</f>
-        <v>45240</v>
+        <v>45327</v>
       </c>
       <c r="AL7" s="99">
         <f ca="1">AK7+1</f>
-        <v>45241</v>
+        <v>45328</v>
       </c>
       <c r="AM7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45242</v>
+        <v>45329</v>
       </c>
       <c r="AN7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45243</v>
+        <v>45330</v>
       </c>
       <c r="AO7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45244</v>
+        <v>45331</v>
       </c>
       <c r="AP7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45245</v>
+        <v>45332</v>
       </c>
       <c r="AQ7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45246</v>
+        <v>45333</v>
       </c>
       <c r="AR7" s="99">
         <f ca="1">AQ7+1</f>
-        <v>45247</v>
+        <v>45334</v>
       </c>
       <c r="AS7" s="99">
         <f ca="1">AR7+1</f>
-        <v>45248</v>
+        <v>45335</v>
       </c>
       <c r="AT7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45249</v>
+        <v>45336</v>
       </c>
       <c r="AU7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45250</v>
+        <v>45337</v>
       </c>
       <c r="AV7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45251</v>
+        <v>45338</v>
       </c>
       <c r="AW7" s="99">
         <f t="shared" ca="1" si="0"/>
-        <v>45252</v>
+        <v>45339</v>
       </c>
       <c r="AX7" s="100">
         <f t="shared" ca="1" si="0"/>
-        <v>45253</v>
+        <v>45340</v>
       </c>
       <c r="AY7" s="99">
         <f ca="1">AX7+1</f>
-        <v>45254</v>
+        <v>45341</v>
       </c>
       <c r="AZ7" s="99">
         <f ca="1">AY7+1</f>
-        <v>45255</v>
+        <v>45342</v>
       </c>
       <c r="BA7" s="99">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45256</v>
+        <v>45343</v>
       </c>
       <c r="BB7" s="99">
         <f t="shared" ca="1" si="1"/>
-        <v>45257</v>
+        <v>45344</v>
       </c>
       <c r="BC7" s="99">
         <f t="shared" ca="1" si="1"/>
-        <v>45258</v>
+        <v>45345</v>
       </c>
       <c r="BD7" s="99">
         <f t="shared" ca="1" si="1"/>
-        <v>45259</v>
+        <v>45346</v>
       </c>
       <c r="BE7" s="100">
         <f t="shared" ca="1" si="1"/>
-        <v>45260</v>
+        <v>45347</v>
       </c>
       <c r="BF7" s="99">
         <f ca="1">BE7+1</f>
-        <v>45261</v>
+        <v>45348</v>
       </c>
       <c r="BG7" s="99">
         <f ca="1">BF7+1</f>
-        <v>45262</v>
+        <v>45349</v>
       </c>
       <c r="BH7" s="99">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45263</v>
+        <v>45350</v>
       </c>
       <c r="BI7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>45264</v>
+        <v>45351</v>
       </c>
       <c r="BJ7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>45265</v>
+        <v>45352</v>
       </c>
       <c r="BK7" s="99">
         <f t="shared" ca="1" si="2"/>
-        <v>45266</v>
+        <v>45353</v>
       </c>
       <c r="BL7" s="100">
         <f t="shared" ca="1" si="2"/>
-        <v>45267</v>
+        <v>45354</v>
       </c>
     </row>
-    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="74"/>
       <c r="C8" s="74"/>
@@ -3590,7 +3572,7 @@
       <c r="BK8" s="102"/>
       <c r="BL8" s="105"/>
     </row>
-    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -3615,230 +3597,230 @@
       <c r="H9" s="88"/>
       <c r="I9" s="106" t="str">
         <f t="shared" ref="I9:AN9" ca="1" si="3">LEFT(TEXT(I7,"TTT"),1)</f>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="J9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="K9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="L9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="M9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="N9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="O9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="P9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="Q9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="R9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="S9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="T9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="U9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="V9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="W9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="X9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="Y9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="Z9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AA9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AB9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AD9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AE9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AF9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AG9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AH9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AI9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AK9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AL9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AM9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AN9" s="106" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AO9" s="106" t="str">
         <f t="shared" ref="AO9:BL9" ca="1" si="4">LEFT(TEXT(AO7,"TTT"),1)</f>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AP9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AR9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AS9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AT9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AU9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AV9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AW9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AY9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AZ9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BA9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BB9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="BC9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="BD9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BF9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BG9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BH9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BI9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="BJ9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="BK9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="106" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
     </row>
-    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="16"/>
       <c r="C10" s="13"/>
       <c r="D10" s="12"/>
@@ -3902,7 +3884,7 @@
       <c r="BK10" s="36"/>
       <c r="BL10" s="36"/>
     </row>
-    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="116" t="s">
         <v>22</v>
@@ -4139,7 +4121,7 @@
       </c>
       <c r="BP11" s="41"/>
     </row>
-    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="63" t="s">
         <v>23</v>
@@ -4155,7 +4137,7 @@
       </c>
       <c r="F12" s="61">
         <f ca="1">TODAY()</f>
-        <v>45211</v>
+        <v>45298</v>
       </c>
       <c r="G12" s="62">
         <v>3</v>
@@ -4386,7 +4368,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="63" t="s">
         <v>26</v>
@@ -4398,7 +4380,7 @@
       <c r="E13" s="60"/>
       <c r="F13" s="61">
         <f ca="1">TODAY()+5</f>
-        <v>45216</v>
+        <v>45303</v>
       </c>
       <c r="G13" s="62">
         <v>1</v>
@@ -4629,7 +4611,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="63" t="s">
         <v>28</v>
@@ -4643,7 +4625,7 @@
       </c>
       <c r="F14" s="61">
         <f ca="1">F12-3</f>
-        <v>45208</v>
+        <v>45295</v>
       </c>
       <c r="G14" s="62">
         <v>10</v>
@@ -4874,7 +4856,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="63" t="s">
         <v>29</v>
@@ -4886,7 +4868,7 @@
       <c r="E15" s="60"/>
       <c r="F15" s="61">
         <f ca="1">F12+20</f>
-        <v>45231</v>
+        <v>45318</v>
       </c>
       <c r="G15" s="62">
         <v>1</v>
@@ -5117,7 +5099,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="63" t="s">
         <v>30</v>
@@ -5131,7 +5113,7 @@
       </c>
       <c r="F16" s="61">
         <f ca="1">F12+6</f>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="G16" s="62">
         <v>6</v>
@@ -5362,7 +5344,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="116" t="s">
         <v>31</v>
@@ -5598,7 +5580,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="63" t="s">
         <v>23</v>
@@ -5612,7 +5594,7 @@
       </c>
       <c r="F18" s="61">
         <f ca="1">F12+6</f>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="G18" s="62">
         <v>13</v>
@@ -5843,7 +5825,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="63" t="s">
         <v>26</v>
@@ -5857,7 +5839,7 @@
       </c>
       <c r="F19" s="61">
         <f ca="1">F18+2</f>
-        <v>45219</v>
+        <v>45306</v>
       </c>
       <c r="G19" s="62">
         <v>9</v>
@@ -6088,7 +6070,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="63" t="s">
         <v>28</v>
@@ -6102,7 +6084,7 @@
       </c>
       <c r="F20" s="61">
         <f ca="1">F19+5</f>
-        <v>45224</v>
+        <v>45311</v>
       </c>
       <c r="G20" s="62">
         <v>11</v>
@@ -6333,7 +6315,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="63" t="s">
         <v>29</v>
@@ -6345,7 +6327,7 @@
       <c r="E21" s="60"/>
       <c r="F21" s="61">
         <f ca="1">F20+2</f>
-        <v>45226</v>
+        <v>45313</v>
       </c>
       <c r="G21" s="62">
         <v>1</v>
@@ -6576,7 +6558,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="63" t="s">
         <v>30</v>
@@ -6586,7 +6568,7 @@
       <c r="E22" s="60"/>
       <c r="F22" s="61">
         <f ca="1">F21+1</f>
-        <v>45227</v>
+        <v>45314</v>
       </c>
       <c r="G22" s="62">
         <v>24</v>
@@ -6817,7 +6799,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="116" t="s">
         <v>33</v>
@@ -7053,7 +7035,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="63" t="s">
         <v>23</v>
@@ -7065,7 +7047,7 @@
       <c r="E24" s="60"/>
       <c r="F24" s="61">
         <f ca="1">F12+15</f>
-        <v>45226</v>
+        <v>45313</v>
       </c>
       <c r="G24" s="62">
         <v>4</v>
@@ -7296,7 +7278,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="63" t="s">
         <v>26</v>
@@ -7308,7 +7290,7 @@
       <c r="E25" s="60"/>
       <c r="F25" s="61">
         <f ca="1">F24+3</f>
-        <v>45229</v>
+        <v>45316</v>
       </c>
       <c r="G25" s="62">
         <v>14</v>
@@ -7539,7 +7521,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="63" t="s">
         <v>28</v>
@@ -7551,7 +7533,7 @@
       <c r="E26" s="60"/>
       <c r="F26" s="61">
         <f ca="1">F25+15</f>
-        <v>45244</v>
+        <v>45331</v>
       </c>
       <c r="G26" s="62">
         <v>6</v>
@@ -7782,7 +7764,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="63" t="s">
         <v>29</v>
@@ -7794,7 +7776,7 @@
       <c r="E27" s="60"/>
       <c r="F27" s="61">
         <f ca="1">F21+22</f>
-        <v>45248</v>
+        <v>45335</v>
       </c>
       <c r="G27" s="62">
         <v>3</v>
@@ -8025,7 +8007,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="63" t="s">
         <v>30</v>
@@ -8037,7 +8019,7 @@
       <c r="E28" s="60"/>
       <c r="F28" s="61">
         <f ca="1">F16</f>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="G28" s="62">
         <v>19</v>
@@ -8268,7 +8250,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="116" t="s">
         <v>34</v>
@@ -8504,7 +8486,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="63" t="s">
         <v>23</v>
@@ -8514,7 +8496,7 @@
       <c r="E30" s="60"/>
       <c r="F30" s="61">
         <f ca="1">F27+3</f>
-        <v>45251</v>
+        <v>45338</v>
       </c>
       <c r="G30" s="62">
         <v>15</v>
@@ -8745,7 +8727,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="63" t="s">
         <v>26</v>
@@ -8755,7 +8737,7 @@
       <c r="E31" s="60"/>
       <c r="F31" s="61">
         <f ca="1">F30+14</f>
-        <v>45265</v>
+        <v>45352</v>
       </c>
       <c r="G31" s="62">
         <v>5</v>
@@ -8986,7 +8968,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="63" t="s">
         <v>28</v>
@@ -8998,7 +8980,7 @@
       <c r="E32" s="60"/>
       <c r="F32" s="61">
         <f ca="1">F31+42</f>
-        <v>45307</v>
+        <v>45394</v>
       </c>
       <c r="G32" s="62">
         <v>1</v>
@@ -9229,7 +9211,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="63" t="s">
         <v>29</v>
@@ -9465,7 +9447,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="63" t="s">
         <v>30</v>
@@ -9701,7 +9683,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="63"/>
       <c r="C35" s="59"/>
@@ -9936,7 +9918,7 @@
       </c>
       <c r="BM35" s="89"/>
     </row>
-    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10"/>
       <c r="B36" s="118" t="s">
         <v>35</v>
@@ -10004,12 +9986,12 @@
       <c r="BK36" s="87"/>
       <c r="BL36" s="87"/>
     </row>
-    <row r="37" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D37" s="4"/>
       <c r="G37" s="11"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D38" s="5"/>
     </row>
   </sheetData>
@@ -10177,22 +10159,22 @@
       <selection activeCell="BO7" sqref="BO7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="64" width="3.5703125" customWidth="1"/>
-    <col min="65" max="65" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" customWidth="1"/>
+    <col min="9" max="64" width="3.54296875" customWidth="1"/>
+    <col min="65" max="65" width="2.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:68" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:68" ht="49.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="136" t="s">
         <v>3</v>
@@ -10261,7 +10243,7 @@
       <c r="BL2" s="20"/>
       <c r="BM2" s="20"/>
     </row>
-    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="42"/>
       <c r="C3" s="43"/>
@@ -10328,7 +10310,7 @@
       <c r="BL3" s="32"/>
       <c r="BM3" s="32"/>
     </row>
-    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="54" t="s">
         <v>4</v>
@@ -10409,7 +10391,7 @@
       <c r="BL4" s="32"/>
       <c r="BM4" s="32"/>
     </row>
-    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -10480,14 +10462,14 @@
       <c r="BL5" s="32"/>
       <c r="BM5" s="32"/>
     </row>
-    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="10"/>
       <c r="B6" s="49" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="34" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">IFERROR(IF(MIN(Meilensteine435[Start])=0,TODAY(),B11(Meilensteine435[Start])),TODAY())</f>
-        <v>45211</v>
+        <v>45298</v>
       </c>
       <c r="D6" s="53"/>
       <c r="E6" s="32"/>
@@ -10496,7 +10478,7 @@
       <c r="H6" s="29"/>
       <c r="I6" s="94" t="str">
         <f ca="1">TEXT(I7,"MMMM")</f>
-        <v>Oktober</v>
+        <v>Januar</v>
       </c>
       <c r="J6" s="94"/>
       <c r="K6" s="94"/>
@@ -10526,7 +10508,7 @@
       <c r="AC6" s="94"/>
       <c r="AD6" s="94" t="str">
         <f ca="1">IF(OR(TEXT(AD7,"MMMM")=W6,TEXT(AD7,"MMMM")=P6,TEXT(AD7,"MMMM")=I6),"",TEXT(AD7,"MMMM"))</f>
-        <v>November</v>
+        <v/>
       </c>
       <c r="AE6" s="94"/>
       <c r="AF6" s="94"/>
@@ -10536,7 +10518,7 @@
       <c r="AJ6" s="94"/>
       <c r="AK6" s="94" t="str">
         <f ca="1">IF(OR(TEXT(AK7,"MMMM")=AD6,TEXT(AK7,"MMMM")=W6,TEXT(AK7,"MMMM")=P6,TEXT(AK7,"MMMM")=I6),"",TEXT(AK7,"MMMM"))</f>
-        <v/>
+        <v>Februar</v>
       </c>
       <c r="AL6" s="94"/>
       <c r="AM6" s="94"/>
@@ -10566,7 +10548,7 @@
       <c r="BE6" s="65"/>
       <c r="BF6" s="65" t="str">
         <f ca="1">IF(OR(TEXT(BF7,"MMMM")=AY6,TEXT(BF7,"MMMM")=AR6,TEXT(BF7,"MMMM")=AK6,TEXT(BF7,"MMMM")=AD6),"",TEXT(BF7,"MMMM"))</f>
-        <v>Dezember</v>
+        <v/>
       </c>
       <c r="BG6" s="65"/>
       <c r="BH6" s="65"/>
@@ -10576,7 +10558,7 @@
       <c r="BL6" s="65"/>
       <c r="BM6" s="32"/>
     </row>
-    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="49" t="s">
         <v>14</v>
@@ -10591,231 +10573,231 @@
       <c r="H7" s="29"/>
       <c r="I7" s="96">
         <f ca="1">IFERROR(Projekt_Start+Scrollschrittweite,TODAY())</f>
-        <v>45212</v>
+        <v>45299</v>
       </c>
       <c r="J7" s="17">
         <f ca="1">I7+1</f>
-        <v>45213</v>
+        <v>45300</v>
       </c>
       <c r="K7" s="17">
         <f t="shared" ref="K7:AX7" ca="1" si="0">J7+1</f>
-        <v>45214</v>
+        <v>45301</v>
       </c>
       <c r="L7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45215</v>
+        <v>45302</v>
       </c>
       <c r="M7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45216</v>
+        <v>45303</v>
       </c>
       <c r="N7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="O7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45218</v>
+        <v>45305</v>
       </c>
       <c r="P7" s="17">
         <f ca="1">O7+1</f>
-        <v>45219</v>
+        <v>45306</v>
       </c>
       <c r="Q7" s="17">
         <f ca="1">P7+1</f>
-        <v>45220</v>
+        <v>45307</v>
       </c>
       <c r="R7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45221</v>
+        <v>45308</v>
       </c>
       <c r="S7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45222</v>
+        <v>45309</v>
       </c>
       <c r="T7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45223</v>
+        <v>45310</v>
       </c>
       <c r="U7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45224</v>
+        <v>45311</v>
       </c>
       <c r="V7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45225</v>
+        <v>45312</v>
       </c>
       <c r="W7" s="17">
         <f ca="1">V7+1</f>
-        <v>45226</v>
+        <v>45313</v>
       </c>
       <c r="X7" s="17">
         <f ca="1">W7+1</f>
-        <v>45227</v>
+        <v>45314</v>
       </c>
       <c r="Y7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45228</v>
+        <v>45315</v>
       </c>
       <c r="Z7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45229</v>
+        <v>45316</v>
       </c>
       <c r="AA7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45230</v>
+        <v>45317</v>
       </c>
       <c r="AB7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45231</v>
+        <v>45318</v>
       </c>
       <c r="AC7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45232</v>
+        <v>45319</v>
       </c>
       <c r="AD7" s="17">
         <f ca="1">AC7+1</f>
-        <v>45233</v>
+        <v>45320</v>
       </c>
       <c r="AE7" s="17">
         <f ca="1">AD7+1</f>
-        <v>45234</v>
+        <v>45321</v>
       </c>
       <c r="AF7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45235</v>
+        <v>45322</v>
       </c>
       <c r="AG7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45236</v>
+        <v>45323</v>
       </c>
       <c r="AH7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45237</v>
+        <v>45324</v>
       </c>
       <c r="AI7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45238</v>
+        <v>45325</v>
       </c>
       <c r="AJ7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45239</v>
+        <v>45326</v>
       </c>
       <c r="AK7" s="17">
         <f ca="1">AJ7+1</f>
-        <v>45240</v>
+        <v>45327</v>
       </c>
       <c r="AL7" s="17">
         <f ca="1">AK7+1</f>
-        <v>45241</v>
+        <v>45328</v>
       </c>
       <c r="AM7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45242</v>
+        <v>45329</v>
       </c>
       <c r="AN7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45243</v>
+        <v>45330</v>
       </c>
       <c r="AO7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45244</v>
+        <v>45331</v>
       </c>
       <c r="AP7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45245</v>
+        <v>45332</v>
       </c>
       <c r="AQ7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45246</v>
+        <v>45333</v>
       </c>
       <c r="AR7" s="17">
         <f ca="1">AQ7+1</f>
-        <v>45247</v>
+        <v>45334</v>
       </c>
       <c r="AS7" s="17">
         <f ca="1">AR7+1</f>
-        <v>45248</v>
+        <v>45335</v>
       </c>
       <c r="AT7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45249</v>
+        <v>45336</v>
       </c>
       <c r="AU7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45250</v>
+        <v>45337</v>
       </c>
       <c r="AV7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45251</v>
+        <v>45338</v>
       </c>
       <c r="AW7" s="17">
         <f t="shared" ca="1" si="0"/>
-        <v>45252</v>
+        <v>45339</v>
       </c>
       <c r="AX7" s="64">
         <f t="shared" ca="1" si="0"/>
-        <v>45253</v>
+        <v>45340</v>
       </c>
       <c r="AY7" s="17">
         <f ca="1">AX7+1</f>
-        <v>45254</v>
+        <v>45341</v>
       </c>
       <c r="AZ7" s="17">
         <f ca="1">AY7+1</f>
-        <v>45255</v>
+        <v>45342</v>
       </c>
       <c r="BA7" s="17">
         <f t="shared" ref="BA7:BE7" ca="1" si="1">AZ7+1</f>
-        <v>45256</v>
+        <v>45343</v>
       </c>
       <c r="BB7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>45257</v>
+        <v>45344</v>
       </c>
       <c r="BC7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>45258</v>
+        <v>45345</v>
       </c>
       <c r="BD7" s="17">
         <f t="shared" ca="1" si="1"/>
-        <v>45259</v>
+        <v>45346</v>
       </c>
       <c r="BE7" s="64">
         <f t="shared" ca="1" si="1"/>
-        <v>45260</v>
+        <v>45347</v>
       </c>
       <c r="BF7" s="17">
         <f ca="1">BE7+1</f>
-        <v>45261</v>
+        <v>45348</v>
       </c>
       <c r="BG7" s="17">
         <f ca="1">BF7+1</f>
-        <v>45262</v>
+        <v>45349</v>
       </c>
       <c r="BH7" s="17">
         <f t="shared" ref="BH7:BL7" ca="1" si="2">BG7+1</f>
-        <v>45263</v>
+        <v>45350</v>
       </c>
       <c r="BI7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>45264</v>
+        <v>45351</v>
       </c>
       <c r="BJ7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>45265</v>
+        <v>45352</v>
       </c>
       <c r="BK7" s="17">
         <f t="shared" ca="1" si="2"/>
-        <v>45266</v>
+        <v>45353</v>
       </c>
       <c r="BL7" s="18">
         <f t="shared" ca="1" si="2"/>
-        <v>45267</v>
+        <v>45354</v>
       </c>
       <c r="BM7" s="32"/>
     </row>
-    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:68" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="51"/>
       <c r="C8" s="51"/>
@@ -10882,7 +10864,7 @@
       <c r="BL8" s="39"/>
       <c r="BM8" s="32"/>
     </row>
-    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:68" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -10907,231 +10889,231 @@
       <c r="H9" s="48"/>
       <c r="I9" s="37" t="str">
         <f t="shared" ref="I9:AN9" ca="1" si="3">LEFT(TEXT(I7,"TTT"),1)</f>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="J9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="K9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="L9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="M9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="N9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="O9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="P9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="Q9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="R9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="S9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="T9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="U9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="V9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="W9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="X9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="Y9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="Z9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AA9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AB9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AC9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AD9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AE9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AF9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AG9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AH9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AI9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AJ9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AK9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AL9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AM9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AN9" s="37" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AO9" s="37" t="str">
         <f t="shared" ref="AO9:BL9" ca="1" si="4">LEFT(TEXT(AO7,"TTT"),1)</f>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AP9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AQ9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AR9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AS9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="AT9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="AU9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="AV9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="AW9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="AX9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="AY9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="AZ9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BA9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BB9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="BC9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="BD9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BE9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BF9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>F</v>
+        <v>M</v>
       </c>
       <c r="BG9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>D</v>
       </c>
       <c r="BH9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>S</v>
+        <v>M</v>
       </c>
       <c r="BI9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>D</v>
       </c>
       <c r="BJ9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>F</v>
       </c>
       <c r="BK9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>M</v>
+        <v>S</v>
       </c>
       <c r="BL9" s="37" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>D</v>
+        <v>S</v>
       </c>
       <c r="BM9" s="32"/>
     </row>
-    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:68" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="16"/>
       <c r="C10" s="13"/>
       <c r="D10" s="12"/>
@@ -11197,7 +11179,7 @@
       <c r="BL10" s="36"/>
       <c r="BM10" s="32"/>
     </row>
-    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="121" t="s">
         <v>22</v>
@@ -11435,7 +11417,7 @@
       <c r="BM11" s="28"/>
       <c r="BP11" s="41"/>
     </row>
-    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="25" t="s">
         <v>23</v>
@@ -11451,7 +11433,7 @@
       </c>
       <c r="F12" s="23">
         <f ca="1">TODAY()</f>
-        <v>45211</v>
+        <v>45298</v>
       </c>
       <c r="G12" s="24">
         <v>3</v>
@@ -11683,7 +11665,7 @@
       </c>
       <c r="BM12" s="28"/>
     </row>
-    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="25" t="s">
         <v>26</v>
@@ -11695,7 +11677,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="23">
         <f ca="1">TODAY()+5</f>
-        <v>45216</v>
+        <v>45303</v>
       </c>
       <c r="G13" s="24">
         <v>1</v>
@@ -11927,7 +11909,7 @@
       </c>
       <c r="BM13" s="28"/>
     </row>
-    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="25" t="s">
         <v>28</v>
@@ -11941,7 +11923,7 @@
       </c>
       <c r="F14" s="23">
         <f ca="1">F12-3</f>
-        <v>45208</v>
+        <v>45295</v>
       </c>
       <c r="G14" s="24">
         <v>10</v>
@@ -12173,7 +12155,7 @@
       </c>
       <c r="BM14" s="28"/>
     </row>
-    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="25" t="s">
         <v>29</v>
@@ -12185,7 +12167,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="23">
         <f ca="1">F12+20</f>
-        <v>45231</v>
+        <v>45318</v>
       </c>
       <c r="G15" s="24">
         <v>1</v>
@@ -12417,7 +12399,7 @@
       </c>
       <c r="BM15" s="28"/>
     </row>
-    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:68" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="25" t="s">
         <v>30</v>
@@ -12431,7 +12413,7 @@
       </c>
       <c r="F16" s="23">
         <f ca="1">F12+6</f>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="G16" s="24">
         <v>6</v>
@@ -12663,7 +12645,7 @@
       </c>
       <c r="BM16" s="28"/>
     </row>
-    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="121" t="s">
         <v>31</v>
@@ -12900,7 +12882,7 @@
       </c>
       <c r="BM17" s="28"/>
     </row>
-    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="25" t="s">
         <v>23</v>
@@ -12914,7 +12896,7 @@
       </c>
       <c r="F18" s="23">
         <f ca="1">F12+6</f>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="G18" s="24">
         <v>13</v>
@@ -13146,7 +13128,7 @@
       </c>
       <c r="BM18" s="28"/>
     </row>
-    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="25" t="s">
         <v>26</v>
@@ -13160,7 +13142,7 @@
       </c>
       <c r="F19" s="23">
         <f ca="1">F18+2</f>
-        <v>45219</v>
+        <v>45306</v>
       </c>
       <c r="G19" s="24">
         <v>9</v>
@@ -13392,7 +13374,7 @@
       </c>
       <c r="BM19" s="28"/>
     </row>
-    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="25" t="s">
         <v>28</v>
@@ -13406,7 +13388,7 @@
       </c>
       <c r="F20" s="23">
         <f ca="1">F19+5</f>
-        <v>45224</v>
+        <v>45311</v>
       </c>
       <c r="G20" s="24">
         <v>11</v>
@@ -13638,7 +13620,7 @@
       </c>
       <c r="BM20" s="28"/>
     </row>
-    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="25" t="s">
         <v>29</v>
@@ -13650,7 +13632,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="23">
         <f ca="1">F20+2</f>
-        <v>45226</v>
+        <v>45313</v>
       </c>
       <c r="G21" s="24">
         <v>1</v>
@@ -13882,7 +13864,7 @@
       </c>
       <c r="BM21" s="28"/>
     </row>
-    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="25" t="s">
         <v>30</v>
@@ -13892,7 +13874,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="23">
         <f ca="1">F21+1</f>
-        <v>45227</v>
+        <v>45314</v>
       </c>
       <c r="G22" s="24">
         <v>24</v>
@@ -14124,7 +14106,7 @@
       </c>
       <c r="BM22" s="28"/>
     </row>
-    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="121" t="s">
         <v>33</v>
@@ -14361,7 +14343,7 @@
       </c>
       <c r="BM23" s="28"/>
     </row>
-    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="25" t="s">
         <v>23</v>
@@ -14373,7 +14355,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="23">
         <f ca="1">F12+15</f>
-        <v>45226</v>
+        <v>45313</v>
       </c>
       <c r="G24" s="24">
         <v>4</v>
@@ -14605,7 +14587,7 @@
       </c>
       <c r="BM24" s="28"/>
     </row>
-    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="25" t="s">
         <v>26</v>
@@ -14617,7 +14599,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="23">
         <f ca="1">F24+3</f>
-        <v>45229</v>
+        <v>45316</v>
       </c>
       <c r="G25" s="24">
         <v>14</v>
@@ -14849,7 +14831,7 @@
       </c>
       <c r="BM25" s="28"/>
     </row>
-    <row r="26" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="25" t="s">
         <v>28</v>
@@ -14861,7 +14843,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="23">
         <f ca="1">F25+15</f>
-        <v>45244</v>
+        <v>45331</v>
       </c>
       <c r="G26" s="24">
         <v>6</v>
@@ -15093,7 +15075,7 @@
       </c>
       <c r="BM26" s="28"/>
     </row>
-    <row r="27" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="25" t="s">
         <v>29</v>
@@ -15105,7 +15087,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="23">
         <f ca="1">F21+22</f>
-        <v>45248</v>
+        <v>45335</v>
       </c>
       <c r="G27" s="24">
         <v>3</v>
@@ -15337,7 +15319,7 @@
       </c>
       <c r="BM27" s="28"/>
     </row>
-    <row r="28" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="25" t="s">
         <v>30</v>
@@ -15349,7 +15331,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="23">
         <f ca="1">F16</f>
-        <v>45217</v>
+        <v>45304</v>
       </c>
       <c r="G28" s="24">
         <v>19</v>
@@ -15581,7 +15563,7 @@
       </c>
       <c r="BM28" s="28"/>
     </row>
-    <row r="29" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="121" t="s">
         <v>34</v>
@@ -15818,7 +15800,7 @@
       </c>
       <c r="BM29" s="28"/>
     </row>
-    <row r="30" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="25" t="s">
         <v>23</v>
@@ -15828,7 +15810,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="23">
         <f ca="1">F27+3</f>
-        <v>45251</v>
+        <v>45338</v>
       </c>
       <c r="G30" s="24">
         <v>15</v>
@@ -16060,7 +16042,7 @@
       </c>
       <c r="BM30" s="28"/>
     </row>
-    <row r="31" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="25" t="s">
         <v>26</v>
@@ -16070,7 +16052,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="23">
         <f ca="1">F30+14</f>
-        <v>45265</v>
+        <v>45352</v>
       </c>
       <c r="G31" s="24">
         <v>5</v>
@@ -16302,7 +16284,7 @@
       </c>
       <c r="BM31" s="28"/>
     </row>
-    <row r="32" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="25" t="s">
         <v>28</v>
@@ -16314,7 +16296,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="23">
         <f ca="1">F31+42</f>
-        <v>45307</v>
+        <v>45394</v>
       </c>
       <c r="G32" s="24">
         <v>1</v>
@@ -16546,7 +16528,7 @@
       </c>
       <c r="BM32" s="28"/>
     </row>
-    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="25" t="s">
         <v>29</v>
@@ -16783,7 +16765,7 @@
       </c>
       <c r="BM33" s="28"/>
     </row>
-    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="25" t="s">
         <v>30</v>
@@ -17020,7 +17002,7 @@
       </c>
       <c r="BM34" s="28"/>
     </row>
-    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="25"/>
       <c r="C35" s="21"/>
@@ -17255,7 +17237,7 @@
       </c>
       <c r="BM35" s="66"/>
     </row>
-    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:65" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10"/>
       <c r="B36" s="117" t="s">
         <v>35</v>
@@ -17324,12 +17306,12 @@
       <c r="BL36" s="56"/>
       <c r="BM36" s="28"/>
     </row>
-    <row r="37" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D37" s="4"/>
       <c r="G37" s="11"/>
       <c r="H37" s="3"/>
     </row>
-    <row r="38" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D38" s="5"/>
     </row>
   </sheetData>
@@ -17493,27 +17475,27 @@
   </sheetPr>
   <dimension ref="A1:JE49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AV4" sqref="AV4"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A14" zoomScale="82" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="2.7109375" customWidth="1"/>
-    <col min="9" max="64" width="3.5703125" customWidth="1"/>
-    <col min="65" max="65" width="22.7109375" hidden="1" customWidth="1"/>
-    <col min="66" max="265" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="37.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="2.7265625" customWidth="1"/>
+    <col min="9" max="64" width="3.54296875" customWidth="1"/>
+    <col min="65" max="65" width="22.7265625" hidden="1" customWidth="1"/>
+    <col min="66" max="265" width="3.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:265" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:265" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:265" ht="25.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:265" ht="49.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="140" t="s">
         <v>36</v>
@@ -17582,7 +17564,7 @@
       <c r="BL2" s="97"/>
       <c r="BM2" s="97"/>
     </row>
-    <row r="3" spans="1:265" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:265" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10"/>
       <c r="B3" s="68"/>
       <c r="C3" s="69"/>
@@ -17596,7 +17578,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10"/>
       <c r="B4" s="72"/>
       <c r="C4" s="73"/>
@@ -17644,7 +17626,7 @@
       <c r="AO4" s="128"/>
       <c r="AP4" s="128"/>
     </row>
-    <row r="5" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -17658,7 +17640,7 @@
       <c r="G5" s="75"/>
       <c r="H5" s="75"/>
     </row>
-    <row r="6" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="10"/>
       <c r="B6" s="79" t="s">
         <v>13</v>
@@ -17980,7 +17962,7 @@
       <c r="JD6" s="91"/>
       <c r="JE6" s="91"/>
     </row>
-    <row r="7" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="79" t="s">
         <v>14</v>
@@ -19022,7 +19004,7 @@
         <v>45458</v>
       </c>
     </row>
-    <row r="8" spans="1:265" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:265" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="10"/>
       <c r="B8" s="74"/>
       <c r="C8" s="74"/>
@@ -19289,7 +19271,7 @@
       <c r="JD8" s="102"/>
       <c r="JE8" s="102"/>
     </row>
-    <row r="9" spans="1:265" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:265" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -20333,7 +20315,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="10" spans="1:265" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:265" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="16"/>
       <c r="C10" s="13"/>
       <c r="D10" s="12"/>
@@ -20598,7 +20580,7 @@
       <c r="JD10" s="36"/>
       <c r="JE10" s="36"/>
     </row>
-    <row r="11" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="116" t="s">
         <v>45</v>
@@ -21638,7 +21620,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10"/>
       <c r="B12" s="63" t="s">
         <v>46</v>
@@ -21648,7 +21630,7 @@
       </c>
       <c r="D12" s="59"/>
       <c r="E12" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="61">
         <v>45202</v>
@@ -22686,7 +22668,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10"/>
       <c r="B13" s="63" t="s">
         <v>47</v>
@@ -22695,7 +22677,9 @@
         <v>6</v>
       </c>
       <c r="D13" s="59"/>
-      <c r="E13" s="60"/>
+      <c r="E13" s="60">
+        <v>1</v>
+      </c>
       <c r="F13" s="61">
         <v>45214</v>
       </c>
@@ -23732,17 +23716,17 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="63" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C14" s="59" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="59"/>
       <c r="E14" s="60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="61">
         <v>45231</v>
@@ -24780,7 +24764,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="63"/>
       <c r="C15" s="59"/>
@@ -25047,7 +25031,7 @@
       <c r="JD15" s="26"/>
       <c r="JE15" s="26"/>
     </row>
-    <row r="16" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="63"/>
       <c r="C16" s="59"/>
@@ -25314,7 +25298,7 @@
       <c r="JD16" s="26"/>
       <c r="JE16" s="26"/>
     </row>
-    <row r="17" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="116" t="s">
         <v>48</v>
@@ -26354,7 +26338,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="63" t="s">
         <v>49</v>
@@ -26364,7 +26348,7 @@
       </c>
       <c r="D18" s="59"/>
       <c r="E18" s="60">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F18" s="61">
         <v>45245</v>
@@ -27402,7 +27386,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="63" t="s">
         <v>50</v>
@@ -27412,7 +27396,7 @@
       </c>
       <c r="D19" s="59"/>
       <c r="E19" s="60">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F19" s="61">
         <v>45245</v>
@@ -28450,7 +28434,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="63" t="s">
         <v>51</v>
@@ -28460,7 +28444,7 @@
       </c>
       <c r="D20" s="59"/>
       <c r="E20" s="60">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F20" s="61">
         <v>45255</v>
@@ -29498,7 +29482,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="63"/>
       <c r="C21" s="59"/>
@@ -29765,7 +29749,7 @@
       <c r="JD21" s="26"/>
       <c r="JE21" s="26"/>
     </row>
-    <row r="22" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="63"/>
       <c r="C22" s="59"/>
@@ -30032,7 +30016,7 @@
       <c r="JD22" s="26"/>
       <c r="JE22" s="26"/>
     </row>
-    <row r="23" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="116" t="s">
         <v>52</v>
@@ -31072,7 +31056,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="63" t="s">
         <v>37</v>
@@ -32112,7 +32096,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="63" t="s">
         <v>53</v>
@@ -33158,7 +33142,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="63" t="s">
         <v>54</v>
@@ -34204,7 +34188,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="63" t="s">
         <v>55</v>
@@ -35250,7 +35234,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="63"/>
       <c r="C28" s="59"/>
@@ -35517,7 +35501,7 @@
       <c r="JD28" s="26"/>
       <c r="JE28" s="26"/>
     </row>
-    <row r="29" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="116" t="s">
         <v>56</v>
@@ -36557,7 +36541,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="63" t="s">
         <v>57</v>
@@ -37603,7 +37587,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="63" t="s">
         <v>58</v>
@@ -38649,7 +38633,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="63"/>
       <c r="C32" s="59"/>
@@ -38916,7 +38900,7 @@
       <c r="JD32" s="26"/>
       <c r="JE32" s="26"/>
     </row>
-    <row r="33" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="63"/>
       <c r="C33" s="59"/>
@@ -39183,7 +39167,7 @@
       <c r="JD33" s="26"/>
       <c r="JE33" s="26"/>
     </row>
-    <row r="34" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="63"/>
       <c r="C34" s="59"/>
@@ -39450,7 +39434,7 @@
       <c r="JD34" s="26"/>
       <c r="JE34" s="26"/>
     </row>
-    <row r="35" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="63"/>
       <c r="C35" s="59"/>
@@ -40488,7 +40472,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:265" s="1" customFormat="1" ht="40.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10"/>
       <c r="B36" s="116" t="s">
         <v>59</v>
@@ -41528,7 +41512,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B37" s="63" t="s">
         <v>60</v>
       </c>
@@ -42573,7 +42557,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="63" t="s">
         <v>61</v>
       </c>
@@ -43618,7 +43602,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="63" t="s">
         <v>62</v>
       </c>
@@ -44663,7 +44647,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B40" s="63" t="s">
         <v>63</v>
       </c>
@@ -45708,7 +45692,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B41" s="63" t="s">
         <v>64</v>
       </c>
@@ -46753,7 +46737,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B42" s="63"/>
       <c r="C42" s="59"/>
       <c r="D42" s="59"/>
@@ -47790,10 +47774,8 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="116" t="s">
-        <v>65</v>
-      </c>
+    <row r="43" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B43" s="116"/>
       <c r="C43" s="59"/>
       <c r="D43" s="59"/>
       <c r="E43" s="60"/>
@@ -48829,19 +48811,13 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="63" t="s">
-        <v>66</v>
-      </c>
+    <row r="44" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="63"/>
       <c r="C44" s="59"/>
       <c r="D44" s="59"/>
       <c r="E44" s="60"/>
-      <c r="F44" s="61">
-        <v>45394</v>
-      </c>
-      <c r="G44" s="62">
-        <v>-28</v>
-      </c>
+      <c r="F44" s="61"/>
+      <c r="G44" s="62"/>
       <c r="H44" s="59"/>
       <c r="I44" s="26" t="str">
         <f t="shared" ca="1" si="207"/>
@@ -49872,20 +49848,13 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="63" t="s">
-        <v>67</v>
-      </c>
+    <row r="45" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="63"/>
       <c r="C45" s="59"/>
       <c r="D45" s="59"/>
       <c r="E45" s="60"/>
-      <c r="F45" s="61">
-        <f t="shared" ref="F45" si="240">F44+14</f>
-        <v>45408</v>
-      </c>
-      <c r="G45" s="62">
-        <v>-35</v>
-      </c>
+      <c r="F45" s="61"/>
+      <c r="G45" s="62"/>
       <c r="H45" s="59"/>
       <c r="I45" s="26" t="str">
         <f t="shared" ca="1" si="239"/>
@@ -50916,22 +50885,13 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="59" t="s">
-        <v>27</v>
-      </c>
+    <row r="46" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="63"/>
+      <c r="C46" s="59"/>
       <c r="D46" s="59"/>
       <c r="E46" s="60"/>
-      <c r="F46" s="61">
-        <f t="shared" ref="F46" si="241">F45+42</f>
-        <v>45450</v>
-      </c>
-      <c r="G46" s="62">
-        <v>-42</v>
-      </c>
+      <c r="F46" s="61"/>
+      <c r="G46" s="62"/>
       <c r="H46" s="59"/>
       <c r="I46" s="26" t="str">
         <f t="shared" ca="1" si="239"/>
@@ -51962,10 +51922,8 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="63" t="s">
-        <v>69</v>
-      </c>
+    <row r="47" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="63"/>
       <c r="C47" s="59"/>
       <c r="D47" s="59"/>
       <c r="E47" s="60"/>
@@ -53001,10 +52959,8 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="63" t="s">
-        <v>70</v>
-      </c>
+    <row r="48" spans="1:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="63"/>
       <c r="C48" s="59"/>
       <c r="D48" s="59"/>
       <c r="E48" s="60"/>
@@ -54040,7 +53996,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:265" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:265" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B49" s="63"/>
       <c r="C49" s="59"/>
       <c r="D49" s="59"/>
@@ -55300,15 +55256,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="25" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e02306daf00165b375dc6a58966960be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df88fb76bf5f555224557953949c1ec9" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -55602,6 +55549,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CD6AD73-D703-40CF-AB8D-72E6A3921BEB}">
   <ds:schemaRefs>
@@ -55615,14 +55571,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E419B9A7-BD90-4E8F-A951-10D5C6932475}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -55641,4 +55589,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAF2F40C-D12E-4644-AA6E-31E499F048DC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>